<commit_message>
Edit PoFDCtAE for refined petroleum products
</commit_message>
<xml_diff>
--- a/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
+++ b/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\OneDrive\Desktop\Input Data for India 2.0\fuels\PoFDCtAE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\fuels\PoFDCtAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341B87E8-56FA-402E-897A-B6B475598ED8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="India data" sheetId="3" r:id="rId2"/>
-    <sheet name="PoFDCtAE" sheetId="2" r:id="rId3"/>
+    <sheet name="Data from BFPIaE" sheetId="4" r:id="rId3"/>
+    <sheet name="PoFDCtAE" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="122">
   <si>
     <t>PoFDCtAE Percentage of Fuel Demand Change that Alters Exports</t>
   </si>
@@ -348,12 +348,66 @@
   </si>
   <si>
     <t>Snapshot - Government Initiatives</t>
+  </si>
+  <si>
+    <t>Start Year Data</t>
+  </si>
+  <si>
+    <t>Converted to BTU</t>
+  </si>
+  <si>
+    <t>Reasoning</t>
+  </si>
+  <si>
+    <t>Fuel</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Imports</t>
+  </si>
+  <si>
+    <t>Exports</t>
+  </si>
+  <si>
+    <t>Domestic Use</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>We estimate the response to a drop in domestic use of a secondary petroleum product by observing how large</t>
+  </si>
+  <si>
+    <t>the export market for that fuel is, versus the domestic use market.  If the fuel's exports are a far larger share</t>
+  </si>
+  <si>
+    <t>BTU</t>
+  </si>
+  <si>
+    <t>of the total outflows (exports + use) than use is, we assume the export market for that fuel can more easily</t>
+  </si>
+  <si>
+    <t>absorb the drop in domestic production.  Where a fuel is more commonly produced for domestic use (where</t>
+  </si>
+  <si>
+    <t>uranium</t>
+  </si>
+  <si>
+    <t>use has a larger share than exports of the total outflows), we assume less of that fuel will be produced, and</t>
+  </si>
+  <si>
+    <t>more crude will be exported instead.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000E+00"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -394,7 +448,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,6 +473,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -433,7 +505,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -470,6 +542,40 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -888,26 +994,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="58.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="64.140625" customWidth="1"/>
+    <col min="2" max="2" width="58.3984375" customWidth="1"/>
+    <col min="3" max="3" width="8.73046875" customWidth="1"/>
+    <col min="4" max="4" width="64.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>100</v>
       </c>
@@ -921,7 +1027,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>78</v>
       </c>
@@ -929,7 +1035,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" s="2">
         <v>2019</v>
       </c>
@@ -937,7 +1043,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>104</v>
       </c>
@@ -945,7 +1051,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
         <v>79</v>
       </c>
@@ -953,13 +1059,13 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" s="3"/>
       <c r="D8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -967,7 +1073,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -975,7 +1081,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -983,7 +1089,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>6</v>
       </c>
@@ -991,7 +1097,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>4</v>
       </c>
@@ -999,7 +1105,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>5</v>
       </c>
@@ -1007,17 +1113,17 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="D16" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1025,7 +1131,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1033,7 +1139,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -1041,7 +1147,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1049,7 +1155,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1057,7 +1163,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1065,7 +1171,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -1073,87 +1179,87 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -1164,7 +1270,7 @@
       <c r="G45" s="18"/>
       <c r="H45" s="18"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -1175,7 +1281,7 @@
       <c r="G46" s="18"/>
       <c r="H46" s="18"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>24</v>
       </c>
@@ -1186,7 +1292,7 @@
       <c r="G47" s="18"/>
       <c r="H47" s="18"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>25</v>
       </c>
@@ -1197,7 +1303,7 @@
       <c r="G48" s="18"/>
       <c r="H48" s="18"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
@@ -1205,7 +1311,7 @@
       <c r="G49" s="18"/>
       <c r="H49" s="18"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" s="12" t="s">
         <v>56</v>
       </c>
@@ -1217,7 +1323,7 @@
       <c r="G50" s="18"/>
       <c r="H50" s="18"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -1228,7 +1334,7 @@
       <c r="G51" s="18"/>
       <c r="H51" s="18"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -1239,7 +1345,7 @@
       <c r="G52" s="18"/>
       <c r="H52" s="18"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -1250,85 +1356,85 @@
       <c r="G53" s="18"/>
       <c r="H53" s="18"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69" s="15" t="s">
         <v>75</v>
       </c>
       <c r="B69" s="16"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70" s="15" t="s">
         <v>73</v>
       </c>
       <c r="B70" s="16"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71" s="15" t="s">
         <v>76</v>
       </c>
       <c r="B71" s="16"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72" s="17" t="s">
         <v>74</v>
       </c>
@@ -1336,7 +1442,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A72" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A72" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1344,31 +1450,31 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3CD7AE-46AC-4156-9B96-F79CEB8B6E80}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A20:A54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A53" s="19" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" s="19" t="s">
         <v>99</v>
       </c>
@@ -1381,26 +1487,499 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="44.1328125" customWidth="1"/>
+    <col min="2" max="5" width="15.3984375" customWidth="1"/>
+    <col min="6" max="6" width="12.86328125" customWidth="1"/>
+    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="100.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22"/>
+      <c r="H2" s="23" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="H3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="29"/>
+      <c r="H4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="30">
+        <v>1.7409687867E+16</v>
+      </c>
+      <c r="C5" s="30">
+        <v>5368030053750000</v>
+      </c>
+      <c r="D5" s="30">
+        <v>38665282500000</v>
+      </c>
+      <c r="E5" s="28">
+        <f t="shared" ref="E5:E24" si="0">B5+C5-D5</f>
+        <v>2.273905263825E+16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" s="31"/>
+      <c r="H5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="30">
+        <v>1175328000</v>
+      </c>
+      <c r="C6" s="30">
+        <v>944568000</v>
+      </c>
+      <c r="D6" s="30">
+        <v>0</v>
+      </c>
+      <c r="E6" s="28">
+        <f t="shared" si="0"/>
+        <v>2119896000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>116</v>
+      </c>
+      <c r="G6" s="31"/>
+      <c r="H6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="30">
+        <v>140502600000000</v>
+      </c>
+      <c r="C7" s="30">
+        <v>275474702176128.06</v>
+      </c>
+      <c r="D7" s="30">
+        <v>0</v>
+      </c>
+      <c r="E7" s="28">
+        <f t="shared" si="0"/>
+        <v>415977302176128.06</v>
+      </c>
+      <c r="F7" t="s">
+        <v>116</v>
+      </c>
+      <c r="G7" s="31"/>
+      <c r="H7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="31"/>
+      <c r="H8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="31"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="31"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="30">
+        <v>3011480623692003.5</v>
+      </c>
+      <c r="C11" s="30">
+        <v>0</v>
+      </c>
+      <c r="D11" s="30">
+        <v>0</v>
+      </c>
+      <c r="E11" s="28">
+        <f t="shared" si="0"/>
+        <v>3011480623692003.5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G11" s="31"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="30">
+        <v>1668106715464803.3</v>
+      </c>
+      <c r="C12" s="30">
+        <v>7681838039669.5898</v>
+      </c>
+      <c r="D12" s="30">
+        <v>619624120038866</v>
+      </c>
+      <c r="E12" s="28">
+        <f t="shared" si="0"/>
+        <v>1056164433465606.8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="31"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="30">
+        <v>4801883515538662</v>
+      </c>
+      <c r="C13" s="30">
+        <v>59899030991783.617</v>
+      </c>
+      <c r="D13" s="30">
+        <v>1313794267340850.5</v>
+      </c>
+      <c r="E13" s="28">
+        <f t="shared" si="0"/>
+        <v>3547988279189595.5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="31"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="30">
+        <v>44278077600000</v>
+      </c>
+      <c r="C14" s="30">
+        <v>0</v>
+      </c>
+      <c r="D14" s="30">
+        <v>0</v>
+      </c>
+      <c r="E14" s="28">
+        <f t="shared" si="0"/>
+        <v>44278077600000</v>
+      </c>
+      <c r="F14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G14" s="31"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="30">
+        <v>11069519400000</v>
+      </c>
+      <c r="C15" s="30">
+        <v>0</v>
+      </c>
+      <c r="D15" s="30">
+        <v>0</v>
+      </c>
+      <c r="E15" s="28">
+        <f t="shared" si="0"/>
+        <v>11069519400000</v>
+      </c>
+      <c r="F15" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="31"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="30">
+        <v>670364225570218.5</v>
+      </c>
+      <c r="C16" s="30">
+        <v>13366862384605.563</v>
+      </c>
+      <c r="D16" s="30">
+        <v>329945609995263.81</v>
+      </c>
+      <c r="E16" s="28">
+        <f t="shared" si="0"/>
+        <v>353785477959560.19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G16" s="31"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="31"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="31"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="30">
+        <v>621866666666666.63</v>
+      </c>
+      <c r="C19" s="30">
+        <v>138666666666.66666</v>
+      </c>
+      <c r="D19" s="30">
+        <v>58666666666.666664</v>
+      </c>
+      <c r="E19" s="28">
+        <f t="shared" si="0"/>
+        <v>621946666666666.63</v>
+      </c>
+      <c r="F19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19" s="31"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="30">
+        <v>1496798572416000</v>
+      </c>
+      <c r="C20" s="30">
+        <v>9910838086572000</v>
+      </c>
+      <c r="D20" s="30">
+        <v>0</v>
+      </c>
+      <c r="E20" s="28">
+        <f t="shared" si="0"/>
+        <v>1.1407636658988E+16</v>
+      </c>
+      <c r="F20" t="s">
+        <v>116</v>
+      </c>
+      <c r="G20" s="31"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="30">
+        <v>401963368680000</v>
+      </c>
+      <c r="C21" s="30">
+        <v>53942585740000</v>
+      </c>
+      <c r="D21" s="30">
+        <v>105596954960000</v>
+      </c>
+      <c r="E21" s="28">
+        <f t="shared" si="0"/>
+        <v>350308999460000</v>
+      </c>
+      <c r="F21" t="s">
+        <v>116</v>
+      </c>
+      <c r="G21" s="31"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="30">
+        <v>554773438980000</v>
+      </c>
+      <c r="C22" s="30">
+        <v>510050992122000</v>
+      </c>
+      <c r="D22" s="30">
+        <v>16087533489000</v>
+      </c>
+      <c r="E22" s="28">
+        <f t="shared" si="0"/>
+        <v>1048736897613000</v>
+      </c>
+      <c r="F22" t="s">
+        <v>116</v>
+      </c>
+      <c r="G22" s="31"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="30">
+        <v>292325783696246.81</v>
+      </c>
+      <c r="C23" s="30">
+        <v>0</v>
+      </c>
+      <c r="D23" s="30">
+        <v>0</v>
+      </c>
+      <c r="E23" s="28">
+        <f t="shared" si="0"/>
+        <v>292325783696246.81</v>
+      </c>
+      <c r="F23" t="s">
+        <v>116</v>
+      </c>
+      <c r="G23" s="31"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="30">
+        <v>0</v>
+      </c>
+      <c r="C24" s="30">
+        <v>0</v>
+      </c>
+      <c r="D24" s="30">
+        <v>0</v>
+      </c>
+      <c r="E24" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>116</v>
+      </c>
+      <c r="G24" s="31"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="22" width="16.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="36.73046875" customWidth="1"/>
+    <col min="2" max="22" width="16.59765625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>72</v>
       </c>
@@ -1468,7 +2047,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
@@ -1536,7 +2115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>36</v>
       </c>
@@ -1604,7 +2183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>37</v>
       </c>
@@ -1672,7 +2251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>38</v>
       </c>
@@ -1740,7 +2319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>39</v>
       </c>
@@ -1808,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>40</v>
       </c>
@@ -1876,7 +2455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>41</v>
       </c>
@@ -1944,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>42</v>
       </c>
@@ -2012,7 +2591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>43</v>
       </c>
@@ -2043,8 +2622,9 @@
       <c r="J10" s="8">
         <v>0</v>
       </c>
-      <c r="K10" s="8">
-        <v>0</v>
+      <c r="K10" s="34">
+        <f>'Data from BFPIaE'!D12/SUM('Data from BFPIaE'!D12:E12)</f>
+        <v>0.36975077717477212</v>
       </c>
       <c r="L10" s="8">
         <v>0</v>
@@ -2080,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>44</v>
       </c>
@@ -2114,8 +2694,9 @@
       <c r="K11" s="8">
         <v>0</v>
       </c>
-      <c r="L11" s="8">
-        <v>0</v>
+      <c r="L11" s="34">
+        <f>'Data from BFPIaE'!D13/SUM('Data from BFPIaE'!D13:E13)</f>
+        <v>0.27022892422007322</v>
       </c>
       <c r="M11" s="8">
         <v>0</v>
@@ -2148,7 +2729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>45</v>
       </c>
@@ -2216,7 +2797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>46</v>
       </c>
@@ -2284,7 +2865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>47</v>
       </c>
@@ -2352,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
         <v>48</v>
       </c>
@@ -2420,7 +3001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
         <v>49</v>
       </c>
@@ -2488,7 +3069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>50</v>
       </c>
@@ -2556,7 +3137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>51</v>
       </c>
@@ -2624,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>52</v>
       </c>
@@ -2692,7 +3273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>53</v>
       </c>
@@ -2760,7 +3341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>54</v>
       </c>
@@ -2828,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>55</v>
       </c>

</xml_diff>